<commit_message>
Updates with Exercise 4 -6
Made changes to exercise 4 to 6.
</commit_message>
<xml_diff>
--- a/data/Lesson4_model.xlsx
+++ b/data/Lesson4_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosai\OET_coding\flex_training\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosai\OET_coding\flex_training_2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8693B2BC-0C74-415D-AAC0-0AD7DC16E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B431858F-56C1-41E5-8F8B-5E5DB5F65313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{FCF45462-9411-4EAA-9E8F-9E8BCD435174}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{FCF45462-9411-4EAA-9E8F-9E8BCD435174}"/>
   </bookViews>
   <sheets>
     <sheet name="snapshots" sheetId="56" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -126,6 +126,48 @@
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Loadshedding Germany</t>
+  </si>
+  <si>
+    <t>loadshedding</t>
+  </si>
+  <si>
+    <t>Solar Germany</t>
+  </si>
+  <si>
+    <t>Gas Germany</t>
+  </si>
+  <si>
+    <t>Germany Demand</t>
+  </si>
+  <si>
+    <t>Wind Germany</t>
+  </si>
+  <si>
+    <t>Germany Battery</t>
   </si>
 </sst>
 </file>
@@ -214,7 +256,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,6 +275,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
@@ -554,10 +597,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -689,6 +732,9 @@
       <c r="A25" s="8">
         <v>42005.958333333336</v>
       </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -702,9 +748,7 @@
   </sheetPr>
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AZ25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -861,7 +905,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -882,37 +926,55 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3">
+        <v>560</v>
+      </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3">
+        <v>300</v>
+      </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
@@ -1039,7 +1101,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1057,8 +1119,12 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3"/>
@@ -1282,7 +1348,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4"/>
@@ -1345,13 +1411,27 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1363,11 +1443,21 @@
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1381,12 +1471,24 @@
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8800</v>
+      </c>
+      <c r="E4" s="3">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.6</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1399,11 +1501,21 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3">
+        <v>80000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2272,10 +2384,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2283,129 +2395,279 @@
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="28.8">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="11">
         <v>42005</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.68290000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="11">
         <v>42005.041666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.68290000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="11">
         <v>42005.083333333336</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.67559999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="11">
         <v>42005.125</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.67510000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="11">
         <v>42005.166666666664</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.67169999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="11">
         <v>42005.208333333336</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.66930000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="11">
         <v>42005.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.65290000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="11">
         <v>42005.291666666664</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.62990000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="11">
         <v>42005.333333333336</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>1.9E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.63429999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="11">
         <v>42005.375</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>2.07E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.64070000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="11">
         <v>42005.416666666664</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="11">
         <v>42005.458333333336</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.59200000000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="11">
         <v>42005.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>0.11269999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.56640000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="11">
         <v>42005.541666666664</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="11">
         <v>42005.583333333336</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.57289999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="11">
         <v>42005.625</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>0.02</v>
+      </c>
+      <c r="C17">
+        <v>0.57540000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="11">
         <v>42005.666666666664</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C18">
+        <v>0.51340000000000008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="11">
         <v>42005.708333333336</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.44699999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="11">
         <v>42005.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0.39570000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="11">
         <v>42005.791666666664</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0.35489999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="11">
         <v>42005.833333333336</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0.31279999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="11">
         <v>42005.875</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0.27080000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="11">
         <v>42005.916666666664</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.23919999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="11">
         <v>42005.958333333336</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0.20879999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2493,8 +2755,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2520,10 +2782,18 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6">
+        <v>55000</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
@@ -2847,10 +3117,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2858,129 +3128,204 @@
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="28.8">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1">
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1">
       <c r="A2" s="10">
         <v>42005</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>39723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="11">
         <v>42005.041666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>39723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="11">
         <v>42005.083333333336</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>38813</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="11">
         <v>42005.125</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>38490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="11">
         <v>42005.166666666664</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>38644</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="11">
         <v>42005.208333333336</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>38773</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="11">
         <v>42005.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>37247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="11">
         <v>42005.291666666664</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>40371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="11">
         <v>42005.333333333336</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="11">
         <v>42005.375</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="11">
         <v>42005.416666666664</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>47101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="11">
         <v>42005.458333333336</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>49603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="11">
         <v>42005.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>49910</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="11">
         <v>42005.541666666664</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>47528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="11">
         <v>42005.583333333336</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>47097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="11">
         <v>42005.625</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>47383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="11">
         <v>42005.666666666664</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>48936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="11">
         <v>42005.708333333336</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>52288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="11">
         <v>42005.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>53367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="11">
         <v>42005.791666666664</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>52599</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="11">
         <v>42005.833333333336</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>50020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="11">
         <v>42005.875</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>48096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="11">
         <v>42005.916666666664</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>47803</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="11">
         <v>42005.958333333336</v>
+      </c>
+      <c r="B25">
+        <v>44876</v>
       </c>
     </row>
   </sheetData>
@@ -3007,8 +3352,8 @@
   </sheetPr>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3054,13 +3399,25 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>

</xml_diff>